<commit_message>
PQD update thu muc unsorted (chua sap xep )
</commit_message>
<xml_diff>
--- a/unsorted/img/mota_duan1.xlsx
+++ b/unsorted/img/mota_duan1.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Vertrigo\www\DuAn1\unsorted\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55107576-2582-420D-8939-170B452106F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -167,12 +168,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -181,7 +182,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -189,7 +190,7 @@
     <font>
       <sz val="10"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -197,7 +198,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -206,7 +207,7 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -219,7 +220,7 @@
     <font>
       <sz val="10"/>
       <color rgb="FF242424"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -272,12 +273,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -338,6 +336,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="8" name="Picture 7" descr="Gợi ý top 15 dầu dưỡng tóc chất lượng nhất nên mua 2023">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tgtFrame="_blank" tooltip="Gợi ý top 15 dầu dưỡng tóc chất lượng nhất nên mua 2023"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -395,6 +398,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="9" name="Picture 8" descr="This article is referenced content from https://chanhtuoi.com - Gợi ý top 15 dầu dưỡng tóc chất lượng nhất nên mua 2023">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3" tgtFrame="_blank" tooltip="This article is referenced content from https://chanhtuoi.com - Gợi ý top 15 dầu dưỡng tóc chất lượng nhất nên mua 2023"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -452,6 +460,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="10" name="Picture 9" descr="Gợi ý top 15 dầu dưỡng tóc chất lượng nhất nên mua 2023">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tgtFrame="_blank" tooltip="Gợi ý top 15 dầu dưỡng tóc chất lượng nhất nên mua 2023"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -509,6 +522,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="11" name="Picture 10" descr="This article is referenced content from https://chanhtuoi.com - Gợi ý top 15 dầu dưỡng tóc chất lượng nhất nên mua 2023">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3" tgtFrame="_blank" tooltip="This article is referenced content from https://chanhtuoi.com - Gợi ý top 15 dầu dưỡng tóc chất lượng nhất nên mua 2023"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -564,7 +582,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1035" name="AutoShape 11" descr="https://www.x-men.com.vn/wp-content/uploads/2022/09/Xmen_Dau-Goi_650g_Water-851x2000.png.webp"/>
+        <xdr:cNvPr id="1035" name="AutoShape 11" descr="https://www.x-men.com.vn/wp-content/uploads/2022/09/Xmen_Dau-Goi_650g_Water-851x2000.png.webp">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -856,33 +880,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="G5:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="106" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="6" width="9" style="3"/>
-    <col min="7" max="7" width="9" style="3" customWidth="1"/>
-    <col min="8" max="8" width="24.25" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13.625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="39.875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="13.75" style="3" customWidth="1"/>
-    <col min="13" max="13" width="11.75" style="3" customWidth="1"/>
-    <col min="14" max="14" width="27.25" style="3" customWidth="1"/>
-    <col min="15" max="15" width="54.625" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="3"/>
+    <col min="1" max="6" width="9" style="2"/>
+    <col min="7" max="7" width="9" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.21875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="39.88671875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.77734375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="11.77734375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="27.21875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="54.6640625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="5" spans="7:19">
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="8" t="s">
         <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -900,367 +924,367 @@
       <c r="N5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="O5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="7:19">
-      <c r="G6" s="10">
-        <v>1</v>
-      </c>
-      <c r="H6" s="10" t="s">
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="3">
-        <v>1</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="3">
-        <v>1</v>
-      </c>
-      <c r="M6" s="3">
-        <v>1</v>
-      </c>
-      <c r="O6" s="3" t="s">
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="7:19">
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>2</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <f>J6+1</f>
         <v>2</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="3">
-        <v>1</v>
-      </c>
-      <c r="M7" s="3">
-        <v>1</v>
-      </c>
-      <c r="O7" s="3" t="s">
+      <c r="L7" s="2">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1</v>
+      </c>
+      <c r="O7" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="7:19">
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <v>3</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <f t="shared" ref="J8:J22" si="0">J7+1</f>
         <v>3</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="3">
-        <v>1</v>
-      </c>
-      <c r="M8" s="3">
-        <v>1</v>
-      </c>
-      <c r="O8" s="3" t="s">
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="7:19">
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>4</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="3">
-        <v>1</v>
-      </c>
-      <c r="M9" s="3">
-        <v>1</v>
-      </c>
-      <c r="O9" s="4" t="s">
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1</v>
+      </c>
+      <c r="O9" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="7:19">
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="J10" s="3">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="J10" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
     </row>
     <row r="11" spans="7:19">
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11" s="2">
         <v>2</v>
       </c>
-      <c r="M11" s="3">
-        <v>1</v>
-      </c>
-      <c r="O11" s="3" t="s">
+      <c r="M11" s="2">
+        <v>1</v>
+      </c>
+      <c r="O11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="7:19">
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="2">
         <v>2</v>
       </c>
-      <c r="M12" s="3">
-        <v>1</v>
-      </c>
-      <c r="O12" s="3" t="s">
+      <c r="M12" s="2">
+        <v>1</v>
+      </c>
+      <c r="O12" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="7:19">
-      <c r="G13" s="11">
-        <v>1</v>
-      </c>
-      <c r="H13" s="11" t="s">
+      <c r="G13" s="10">
+        <v>1</v>
+      </c>
+      <c r="H13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13" s="2">
         <v>2</v>
       </c>
-      <c r="M13" s="3">
-        <v>1</v>
-      </c>
-      <c r="O13" s="3" t="s">
+      <c r="M13" s="2">
+        <v>1</v>
+      </c>
+      <c r="O13" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="7:19">
-      <c r="G14" s="11">
+      <c r="G14" s="10">
         <f>G13+1</f>
         <v>2</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="K14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14" s="2">
         <v>2</v>
       </c>
-      <c r="M14" s="3">
-        <v>1</v>
-      </c>
-      <c r="O14" s="3" t="s">
+      <c r="M14" s="2">
+        <v>1</v>
+      </c>
+      <c r="O14" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="7:19">
-      <c r="G15" s="11">
+      <c r="G15" s="10">
         <f t="shared" ref="G15:G17" si="1">G14+1</f>
         <v>3</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
     </row>
     <row r="16" spans="7:19">
-      <c r="G16" s="11">
+      <c r="G16" s="10">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16" s="2">
         <v>4</v>
       </c>
-      <c r="M16" s="3">
+      <c r="M16" s="2">
         <v>3</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="O16" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="7:15" ht="25.5">
-      <c r="G17" s="11">
+    <row r="17" spans="7:15" ht="27.6">
+      <c r="G17" s="10">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="J17" s="3">
+      <c r="H17" s="10"/>
+      <c r="J17" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L17" s="3">
+      <c r="L17" s="2">
         <v>4</v>
       </c>
-      <c r="M17" s="3">
+      <c r="M17" s="2">
         <v>3</v>
       </c>
-      <c r="O17" s="4" t="s">
+      <c r="O17" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="7:15">
-      <c r="J18" s="3">
+    <row r="18" spans="7:15" ht="26.4">
+      <c r="J18" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="K18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18" s="2">
         <v>4</v>
       </c>
-      <c r="M18" s="3">
-        <v>5</v>
-      </c>
-      <c r="O18" s="3" t="s">
+      <c r="M18" s="2">
+        <v>3</v>
+      </c>
+      <c r="O18" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="7:15">
-      <c r="J19" s="3">
+      <c r="J19" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="7:15">
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="K20" s="13" t="s">
+      <c r="K20" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20" s="2">
         <v>3</v>
       </c>
-      <c r="M20" s="3">
-        <v>1</v>
-      </c>
-      <c r="O20" s="3" t="s">
+      <c r="M20" s="2">
+        <v>1</v>
+      </c>
+      <c r="O20" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="7:15">
-      <c r="J21" s="3">
+      <c r="J21" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="K21" s="12" t="s">
+      <c r="K21" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21" s="2">
         <v>3</v>
       </c>
-      <c r="M21" s="3">
-        <v>1</v>
-      </c>
-      <c r="O21" s="3" t="s">
+      <c r="M21" s="2">
+        <v>1</v>
+      </c>
+      <c r="O21" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="7:15">
-      <c r="J22" s="3">
+      <c r="J22" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="K22" s="12" t="s">
+      <c r="K22" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="L22" s="3">
+      <c r="L22" s="2">
         <v>3</v>
       </c>
-      <c r="M22" s="3">
-        <v>1</v>
-      </c>
-      <c r="O22" s="3" t="s">
+      <c r="M22" s="2">
+        <v>1</v>
+      </c>
+      <c r="O22" s="2" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K16" r:id="rId1" display="https://vn.moroccanoil.com/products/intense-hydrating-mask"/>
-    <hyperlink ref="K17" r:id="rId2" display="https://vn.moroccanoil.com/products/moroccanoil-treatment-original"/>
-    <hyperlink ref="O17" r:id="rId3"/>
-    <hyperlink ref="O9" r:id="rId4"/>
+    <hyperlink ref="K16" r:id="rId1" display="https://vn.moroccanoil.com/products/intense-hydrating-mask" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K17" r:id="rId2" display="https://vn.moroccanoil.com/products/moroccanoil-treatment-original" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="O17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="O9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>